<commit_message>
Unit update to RMSE table. RMSE output is in units of model output.
</commit_message>
<xml_diff>
--- a/RMSE Table.xlsx
+++ b/RMSE Table.xlsx
@@ -42,10 +42,10 @@
     <t>Vanern</t>
   </si>
   <si>
-    <t>DO RMSE ((mg/L)^2)</t>
-  </si>
-  <si>
-    <t>DOC RMSE ((mg/L)^2)</t>
+    <t>DO RMSE (mg/L)</t>
+  </si>
+  <si>
+    <t>DOC RMSE (mg/L)</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>